<commit_message>
Parte Editar solo falta con peliculas
</commit_message>
<xml_diff>
--- a/reporte.xlsx
+++ b/reporte.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MEGA\MEGASync\NetBeansProjects\PruebaNetbeans\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MEGA\MEGASync\NetBeansProjects\PruebaNetbeans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{2F86524B-C317-44AC-A701-D009C62AC3B5}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34"/>
+  <xr:revisionPtr documentId="13_ncr:1_{BF2F99CE-FD83-42F4-9E7C-2B253C97BD0E}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34"/>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="12225" windowWidth="28800" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
+    <workbookView activeTab="5" windowHeight="12225" windowWidth="28800" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Nombre Pelicula" r:id="rId1" sheetId="6"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>Nombre Pelicula</t>
   </si>
@@ -57,21 +57,6 @@
     <t>Accion</t>
   </si>
   <si>
-    <t>sd</t>
-  </si>
-  <si>
-    <t>dadas</t>
-  </si>
-  <si>
-    <t>adasd</t>
-  </si>
-  <si>
-    <t>adad</t>
-  </si>
-  <si>
-    <t>dasda</t>
-  </si>
-  <si>
     <t>Rey Leon</t>
   </si>
   <si>
@@ -84,16 +69,28 @@
     <t>Nota</t>
   </si>
   <si>
-    <t>1895</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>1888</t>
-  </si>
-  <si>
-    <t>4</t>
+    <t>Liliana te quiero mucho</t>
+  </si>
+  <si>
+    <t>Romantico</t>
+  </si>
+  <si>
+    <t>EEUU</t>
+  </si>
+  <si>
+    <t>BabysTooMuch</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Carlos</t>
   </si>
 </sst>
 </file>
@@ -130,8 +127,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -446,11 +444,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="265" zoomScaleNormal="265">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.0" collapsed="false"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -469,12 +472,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -484,11 +482,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="280" zoomScaleNormal="280">
+      <selection activeCell="A4" sqref="A3:A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="false"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -502,12 +505,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -517,9 +515,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="325" zoomScaleNormal="325">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -535,17 +535,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -555,9 +550,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="295" zoomScaleNormal="295">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -573,12 +570,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -588,11 +580,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="235" zoomScaleNormal="235">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625" collapsed="false"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -606,17 +603,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -626,16 +618,24 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="295" zoomScaleNormal="295">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="22.0" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.140625" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="5.5703125" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.28515625" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="5.140625" collapsed="false"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -651,56 +651,33 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corregida parte editar y añadido mensajes de aviso (correcto, error)
</commit_message>
<xml_diff>
--- a/reporte.xlsx
+++ b/reporte.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="58">
   <si>
     <t>Nombre Pelicula</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>Francis Ford Coppola3</t>
+  </si>
+  <si>
+    <t>Testigo de cargoz</t>
+  </si>
+  <si>
+    <t>Documental</t>
   </si>
 </sst>
 </file>
@@ -229,7 +235,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -295,6 +301,16 @@
         <v>3</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -302,7 +318,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -331,6 +347,16 @@
     <row r="5">
       <c r="A5" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -484,7 +510,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -518,7 +544,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
@@ -741,6 +767,29 @@
       </c>
       <c r="G11" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corregida fallo volver y corregidos nombres
</commit_message>
<xml_diff>
--- a/reporte.xlsx
+++ b/reporte.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="59">
   <si>
     <t>Nombre Pelicula</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>Documental</t>
+  </si>
+  <si>
+    <t>8.75</t>
   </si>
 </sst>
 </file>
@@ -559,7 +562,7 @@
         <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Corregido fallo eliminar Pelicula, añadido mensaje de si desea realizar la acción y corregido control de jtext
</commit_message>
<xml_diff>
--- a/reporte.xlsx
+++ b/reporte.xlsx
@@ -1,23 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MEGA\MEGASync\NetBeansProjects\PruebaNetbeans\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr documentId="13_ncr:1_{EE0B11F1-5663-49CD-B267-994B4BC7E36E}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView windowHeight="8850" windowWidth="20040" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Nombre Pelicula" r:id="rId3" sheetId="1"/>
-    <sheet name="Genero" r:id="rId4" sheetId="2"/>
-    <sheet name="Director" r:id="rId5" sheetId="3"/>
-    <sheet name="Pais" r:id="rId6" sheetId="4"/>
-    <sheet name="Productor" r:id="rId7" sheetId="5"/>
-    <sheet name="Pelicula" r:id="rId8" sheetId="6"/>
+    <sheet name="Nombre Pelicula" r:id="rId1" sheetId="1"/>
+    <sheet name="Genero" r:id="rId2" sheetId="2"/>
+    <sheet name="Director" r:id="rId3" sheetId="3"/>
+    <sheet name="Pais" r:id="rId4" sheetId="4"/>
+    <sheet name="Productor" r:id="rId5" sheetId="5"/>
+    <sheet name="Pelicula" r:id="rId6" sheetId="6"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="58">
   <si>
     <t>Nombre Pelicula</t>
   </si>
@@ -181,29 +189,26 @@
     <t>8.5</t>
   </si>
   <si>
-    <t>El Padrino4</t>
-  </si>
-  <si>
-    <t>Francis Ford Coppola3</t>
-  </si>
-  <si>
-    <t>Testigo de cargoz</t>
-  </si>
-  <si>
     <t>Documental</t>
   </si>
   <si>
     <t>8.75</t>
+  </si>
+  <si>
+    <t>Testigo de cargo2</t>
+  </si>
+  <si>
+    <t>Francis Ford Coppola2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -215,7 +220,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -233,85 +238,385 @@
   <cellXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr lastClr="000000" val="windowText"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -320,46 +625,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -368,54 +673,54 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -426,24 +731,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -454,54 +759,54 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -512,14 +817,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,15 +850,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
         <v>28</v>
@@ -559,38 +867,38 @@
         <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -605,194 +913,194 @@
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
         <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
         <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
         <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
         <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
         <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G12" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arreglado bug en eliminar
</commit_message>
<xml_diff>
--- a/reporte.xlsx
+++ b/reporte.xlsx
@@ -626,7 +626,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -660,11 +660,6 @@
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>